<commit_message>
Add data for testing multiple leagues
</commit_message>
<xml_diff>
--- a/TheScoreTest/src/test/java/TheScore/TheScoreTest/TheScoreData.xlsx
+++ b/TheScoreTest/src/test/java/TheScore/TheScoreTest/TheScoreData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB4837A-B463-401E-8462-B3BF2FFF3417}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7F933F-5266-45CA-8866-3407CD66D8DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>deviceName</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>NFL Football</t>
+  </si>
+  <si>
+    <t>CFL Football</t>
+  </si>
+  <si>
+    <t>MLB Baseball</t>
   </si>
 </sst>
 </file>
@@ -395,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +457,46 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>